<commit_message>
more words processed, added information to console about the count of words
</commit_message>
<xml_diff>
--- a/usefull-projects/subtitles/excel-export/excel/iknow.xlsx
+++ b/usefull-projects/subtitles/excel-export/excel/iknow.xlsx
@@ -1,25 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
-  </bookViews>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="English words" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="English words" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="558">
   <si>
     <t>now</t>
   </si>
@@ -555,18 +547,12 @@
     <t>say</t>
   </si>
   <si>
-    <t>"get</t>
-  </si>
-  <si>
-    <t>advice"</t>
+    <t>advice</t>
   </si>
   <si>
     <t>because</t>
   </si>
   <si>
-    <t>advice</t>
-  </si>
-  <si>
     <t>api</t>
   </si>
   <si>
@@ -624,12 +610,6 @@
     <t>yeah</t>
   </si>
   <si>
-    <t>"hello</t>
-  </si>
-  <si>
-    <t>world"</t>
-  </si>
-  <si>
     <t>beautiful</t>
   </si>
   <si>
@@ -945,12 +925,6 @@
     <t>says</t>
   </si>
   <si>
-    <t>"you</t>
-  </si>
-  <si>
-    <t>read"</t>
-  </si>
-  <si>
     <t>any</t>
   </si>
   <si>
@@ -1231,26 +1205,499 @@
   </si>
   <si>
     <t>why</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>let</t>
+  </si>
+  <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>quick</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>important</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>students</t>
+  </si>
+  <si>
+    <t>never</t>
+  </si>
+  <si>
+    <t>written</t>
+  </si>
+  <si>
+    <t>their</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>better</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>everyone</t>
+  </si>
+  <si>
+    <t>types</t>
+  </si>
+  <si>
+    <t>welcome</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>progressing</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>fast</t>
+  </si>
+  <si>
+    <t>perfect</t>
+  </si>
+  <si>
+    <t>rewatch</t>
+  </si>
+  <si>
+    <t>lectures</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>sections</t>
+  </si>
+  <si>
+    <t>watch</t>
+  </si>
+  <si>
+    <t>slower</t>
+  </si>
+  <si>
+    <t>faster</t>
+  </si>
+  <si>
+    <t>playback</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>questions</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>one-star</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>couple</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>entire</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>parts</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>practice</t>
+  </si>
+  <si>
+    <t>learned</t>
+  </si>
+  <si>
+    <t>videos</t>
+  </si>
+  <si>
+    <t>allow</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>half</t>
+  </si>
+  <si>
+    <t>taking</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>wrote</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>ready</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>recorded</t>
+  </si>
+  <si>
+    <t>mac</t>
+  </si>
+  <si>
+    <t>windows</t>
+  </si>
+  <si>
+    <t>linux</t>
+  </si>
+  <si>
+    <t>computer</t>
+  </si>
+  <si>
+    <t>operating</t>
+  </si>
+  <si>
+    <t>must</t>
+  </si>
+  <si>
+    <t>finally</t>
+  </si>
+  <si>
+    <t>much</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>feeling</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>doing</t>
+  </si>
+  <si>
+    <t>starting</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>download</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>located</t>
+  </si>
+  <si>
+    <t>repository</t>
+  </si>
+  <si>
+    <t>resources</t>
+  </si>
+  <si>
+    <t>access</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>desktop</t>
+  </si>
+  <si>
+    <t>macos</t>
+  </si>
+  <si>
+    <t>double-clicking</t>
+  </si>
+  <si>
+    <t>right-click</t>
+  </si>
+  <si>
+    <t>somewhere</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>finished</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>cannot</t>
+  </si>
+  <si>
+    <t>fix</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>updates-and-fixes</t>
+  </si>
+  <si>
+    <t>fixes</t>
+  </si>
+  <si>
+    <t>catch</t>
+  </si>
+  <si>
+    <t>future</t>
+  </si>
+  <si>
+    <t>asked</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>them</t>
+  </si>
+  <si>
+    <t>versions</t>
+  </si>
+  <si>
+    <t>template</t>
+  </si>
+  <si>
+    <t>promise</t>
+  </si>
+  <si>
+    <t>leaving</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>sitting</t>
+  </si>
+  <si>
+    <t>yourself</t>
+  </si>
+  <si>
+    <t>typing</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>few</t>
+  </si>
+  <si>
+    <t>things</t>
+  </si>
+  <si>
+    <t>best</t>
+  </si>
+  <si>
+    <t>fundamentals</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>trying</t>
+  </si>
+  <si>
+    <t>solve</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>can't</t>
+  </si>
+  <si>
+    <t>checking</t>
+  </si>
+  <si>
+    <t>diving</t>
+  </si>
+  <si>
+    <t>someone</t>
+  </si>
+  <si>
+    <t>had</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>previous</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>moving</t>
+  </si>
+  <si>
+    <t>possible</t>
+  </si>
+  <si>
+    <t>own</t>
+  </si>
+  <si>
+    <t>importantly</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>includes</t>
+  </si>
+  <si>
+    <t>exercises</t>
+  </si>
+  <si>
+    <t>without</t>
+  </si>
+  <si>
+    <t>such</t>
+  </si>
+  <si>
+    <t>apps</t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>soft</t>
+  </si>
+  <si>
+    <t>music</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1273,14 +1720,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1296,9 +1740,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1306,44 +1750,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1373,12 +1817,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1408,7 +1852,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1417,2179 +1861,3001 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A404"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
+  <dimension ref="A1:A558"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="1" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="1" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="1" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="1" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="1" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="1" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="1" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="1" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="1" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A82" s="1" t="s">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="1" t="s">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="1" t="s">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A88" s="1" t="s">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A90" s="1" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A92" s="1" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A94" s="1" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A95" s="1" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A97" s="1" t="s">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A98" s="1" t="s">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A99" s="1" t="s">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A101" s="1" t="s">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A102" s="1" t="s">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="1" t="s">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A105" s="1" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A106" s="1" t="s">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A107" s="1" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A109" s="1" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A110" s="1" t="s">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A111" s="1" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A112" s="1" t="s">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A113" s="1" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A114" s="1" t="s">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A115" s="1" t="s">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A116" s="1" t="s">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A117" s="1" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A118" s="1" t="s">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A119" s="1" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A120" s="1" t="s">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A121" s="1" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A122" s="1" t="s">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A124" s="1" t="s">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A125" s="1" t="s">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A126" s="1" t="s">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A127" s="1" t="s">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A128" s="1" t="s">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A129" s="1" t="s">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A130" s="1" t="s">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A131" s="1" t="s">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A132" s="1" t="s">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A133" s="1" t="s">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A134" s="1" t="s">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A135" s="1" t="s">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A136" s="1" t="s">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A137" s="1" t="s">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A138" s="1" t="s">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A139" s="1" t="s">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A140" s="1" t="s">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A141" s="1" t="s">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A142" s="1" t="s">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A143" s="1" t="s">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A144" s="1" t="s">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A145" s="1" t="s">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A146" s="1" t="s">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A147" s="1" t="s">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A148" s="1" t="s">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A149" s="1" t="s">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A150" s="1" t="s">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A151" s="1" t="s">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A153" s="1" t="s">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A154" s="1" t="s">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A155" s="1" t="s">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="157" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A158" s="1" t="s">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A159" s="1" t="s">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A160" s="1" t="s">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="161" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A161" s="1" t="s">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A162" s="1" t="s">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A163" s="1" t="s">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A164" s="1" t="s">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A165" s="1" t="s">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A166" s="1" t="s">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A167" s="1" t="s">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A168" s="1" t="s">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A169" s="1" t="s">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A170" s="1" t="s">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A171" s="1" t="s">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A172" s="1" t="s">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A173" s="1" t="s">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A174" s="1" t="s">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A175" s="1" t="s">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A176" s="1" t="s">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A177" s="1" t="s">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A178" s="1" t="s">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A179" s="1" t="s">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A180" s="1" t="s">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A181" s="1" t="s">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A182" s="1" t="s">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A183" s="1" t="s">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A184" s="1" t="s">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A185" s="1" t="s">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A186" s="1" t="s">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A187" s="1" t="s">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A188" s="1" t="s">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A189" s="1" t="s">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A190" s="1" t="s">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A191" s="1" t="s">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A192" s="1" t="s">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A193" s="1" t="s">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="194" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A194" s="1" t="s">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="195" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A195" s="1" t="s">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A196" s="1" t="s">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A197" s="1" t="s">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A198" s="1" t="s">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A199" s="1" t="s">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A200" s="1" t="s">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A201" s="1" t="s">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="202" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A202" s="1" t="s">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="203" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A203" s="1" t="s">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A204" s="1" t="s">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="205" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A205" s="1" t="s">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A206" s="1" t="s">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="207" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A207" s="1" t="s">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="208" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A208" s="1" t="s">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A209" s="1" t="s">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A210" s="1" t="s">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A211" s="1" t="s">
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A212" s="1" t="s">
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A213" s="1" t="s">
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A214" s="1" t="s">
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A215" s="1" t="s">
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A216" s="1" t="s">
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A217" s="1" t="s">
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A218" s="1" t="s">
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A219" s="1" t="s">
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A220" s="1" t="s">
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A221" s="1" t="s">
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="222" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A222" s="1" t="s">
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="223" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A223" s="1" t="s">
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A224" s="1" t="s">
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A225" s="1" t="s">
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A226" s="1" t="s">
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A227" s="1" t="s">
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A228" s="1" t="s">
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A229" s="1" t="s">
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A230" s="1" t="s">
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A231" s="1" t="s">
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A232" s="1" t="s">
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A233" s="1" t="s">
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A234" s="1" t="s">
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="235" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A235" s="1" t="s">
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="236" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A236" s="1" t="s">
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="237" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A237" s="1" t="s">
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="238" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A238" s="1" t="s">
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="239" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A239" s="1" t="s">
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A240" s="1" t="s">
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A241" s="1" t="s">
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="242" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A242" s="1" t="s">
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A243" s="1" t="s">
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A244" s="1" t="s">
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A245" s="1" t="s">
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A246" s="1" t="s">
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A247" s="1" t="s">
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A248" s="1" t="s">
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="249" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A249" s="1" t="s">
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A250" s="1" t="s">
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A251" s="1" t="s">
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A252" s="1" t="s">
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A253" s="1" t="s">
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A254" s="1" t="s">
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A255" s="1" t="s">
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A256" s="1" t="s">
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A257" s="1" t="s">
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A258" s="1" t="s">
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A259" s="1" t="s">
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A260" s="1" t="s">
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A261" s="1" t="s">
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A262" s="1" t="s">
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A263" s="1" t="s">
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="264" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A264" s="1" t="s">
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A265" s="1" t="s">
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A266" s="1" t="s">
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A267" s="1" t="s">
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A268" s="1" t="s">
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A269" s="1" t="s">
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A270" s="1" t="s">
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A271" s="1" t="s">
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A272" s="1" t="s">
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="273" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A273" s="1" t="s">
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="274" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A274" s="1" t="s">
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="275" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A275" s="1" t="s">
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="276" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A276" s="1" t="s">
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="277" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A277" s="1" t="s">
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="278" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A278" s="1" t="s">
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="279" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A279" s="1" t="s">
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="280" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A280" s="1" t="s">
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="281" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A281" s="1" t="s">
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="282" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A282" s="1" t="s">
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="283" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A283" s="1" t="s">
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="284" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A284" s="1" t="s">
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="285" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A285" s="1" t="s">
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="286" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A286" s="1" t="s">
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="287" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A287" s="1" t="s">
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="288" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A288" s="1" t="s">
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A289" s="1" t="s">
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A290" s="1" t="s">
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A291" s="1" t="s">
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A292" s="1" t="s">
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A293" s="1" t="s">
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A294" s="1" t="s">
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A295" s="1" t="s">
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A296" s="1" t="s">
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A297" s="1" t="s">
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A298" s="1" t="s">
+    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A299" s="1" t="s">
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A300" s="1" t="s">
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="301" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A301" s="1" t="s">
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A302" s="1" t="s">
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A303" s="1" t="s">
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A304" s="1" t="s">
+    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="305" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A305" s="1" t="s">
+    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="306" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A306" s="1" t="s">
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="307" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A307" s="1" t="s">
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="308" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A308" s="1" t="s">
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="309" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A309" s="1" t="s">
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="310" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A310" s="1" t="s">
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="311" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A311" s="1" t="s">
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="312" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A312" s="1" t="s">
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="313" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A313" s="1" t="s">
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="314" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A314" s="1" t="s">
+    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="315" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A315" s="1" t="s">
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="316" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A316" s="1" t="s">
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="317" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A317" s="1" t="s">
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="318" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A318" s="1" t="s">
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="319" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A319" s="1" t="s">
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="320" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A320" s="1" t="s">
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="321" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A321" s="1" t="s">
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="322" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A322" s="1" t="s">
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="323" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A323" s="1" t="s">
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="324" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A324" s="1" t="s">
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="325" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A325" s="1" t="s">
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="326" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A326" s="1" t="s">
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="327" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A327" s="1" t="s">
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="328" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A328" s="1" t="s">
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="329" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A329" s="1" t="s">
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="330" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A330" s="1" t="s">
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="331" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A331" s="1" t="s">
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="332" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A332" s="1" t="s">
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="333" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A333" s="1" t="s">
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="334" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A334" s="1" t="s">
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="335" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A335" s="1" t="s">
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="336" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A336" s="1" t="s">
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="337" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A337" s="1" t="s">
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="338" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A338" s="1" t="s">
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="339" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A339" s="1" t="s">
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="340" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A340" s="1" t="s">
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="341" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A341" s="1" t="s">
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="342" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A342" s="1" t="s">
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="343" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A343" s="1" t="s">
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="344" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A344" s="1" t="s">
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="345" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A345" s="1" t="s">
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="346" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A346" s="1" t="s">
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="347" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A347" s="1" t="s">
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A348" s="1" t="s">
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="349" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A349" s="1" t="s">
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="350" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A350" s="1" t="s">
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="351" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A351" s="1" t="s">
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="352" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A352" s="1" t="s">
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="353" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A353" s="1" t="s">
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="354" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A354" s="1" t="s">
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="355" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A355" s="1" t="s">
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="356" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A356" s="1" t="s">
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="357" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A357" s="1" t="s">
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="358" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A358" s="1" t="s">
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="359" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A359" s="1" t="s">
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="360" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A360" s="1" t="s">
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="361" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A361" s="1" t="s">
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="362" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A362" s="1" t="s">
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="363" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A363" s="1" t="s">
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="364" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A364" s="1" t="s">
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="365" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A365" s="1" t="s">
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="366" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A366" s="1" t="s">
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="367" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A367" s="1" t="s">
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="368" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A368" s="1" t="s">
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="369" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A369" s="1" t="s">
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="370" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A370" s="1" t="s">
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="371" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A371" s="1" t="s">
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="372" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A372" s="1" t="s">
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="373" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A373" s="1" t="s">
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="374" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A374" s="1" t="s">
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="375" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A375" s="1" t="s">
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="376" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A376" s="1" t="s">
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="377" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A377" s="1" t="s">
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="378" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A378" s="1" t="s">
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="379" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A379" s="1" t="s">
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="380" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A380" s="1" t="s">
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="381" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A381" s="1" t="s">
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="382" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A382" s="1" t="s">
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="383" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A383" s="1" t="s">
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="384" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A384" s="1" t="s">
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="385" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A385" s="1" t="s">
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="386" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A386" s="1" t="s">
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="387" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A387" s="1" t="s">
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="388" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A388" s="1" t="s">
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="389" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A389" s="1" t="s">
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="390" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A390" s="1" t="s">
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="391" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A391" s="1" t="s">
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="392" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A392" s="1" t="s">
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="393" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A393" s="1" t="s">
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="394" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A394" s="1" t="s">
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="395" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A395" s="1" t="s">
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="396" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A396" s="1" t="s">
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="397" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A397" s="1" t="s">
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="398" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A398" s="1" t="s">
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="399" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A399" s="1" t="s">
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A400" s="1" t="s">
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="401" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A401" s="1" t="s">
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A402" s="1" t="s">
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="403" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A403" s="1" t="s">
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="404" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A404" s="1" t="s">
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
         <v>403</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>557</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>